<commit_message>
bug fix in pf result creation; updated pf result files
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_ward34_impedance.xlsx
+++ b/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_ward34_impedance.xlsx
@@ -740,13 +740,13 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
@@ -761,7 +761,7 @@
         <v>0.9526279647833882</v>
       </c>
       <c r="Q2">
-        <v>-8.692030605078384E-11</v>
+        <v>-8.69272151632366E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -811,16 +811,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9526279646671955</v>
+        <v>0.9526279646671957</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.9526279648965608</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>1.457878492964093E-10</v>
+        <v>1.457724166160542E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -870,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279646404242</v>
+        <v>0.9526279646404244</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279649233321</v>
+        <v>0.9526279649233318</v>
       </c>
       <c r="Q4">
-        <v>1.564915676528601E-09</v>
+        <v>1.564897976846374E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -929,22 +929,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9526279646315002</v>
+        <v>0.9526279646315007</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279649322559</v>
+        <v>0.9526279649322554</v>
       </c>
       <c r="Q5">
-        <v>2.037958276970909E-09</v>
+        <v>2.037934891115733E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999979535</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -988,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9526279646315001</v>
+        <v>0.9526279646315007</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.9526279649322557</v>
+        <v>0.9526279649322554</v>
       </c>
       <c r="Q6">
-        <v>2.03795072457894E-09</v>
+        <v>2.037934891115733E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1086,19 +1086,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.734156921377197</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="D2">
-        <v>3.734156921377197</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>237.1508154128772</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="G2">
-        <v>237.1508154128772</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="H2">
         <v>1.324394477419386</v>
@@ -1107,13 +1107,13 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
@@ -1128,7 +1128,7 @@
         <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884997137</v>
+        <v>5.766209884997138</v>
       </c>
       <c r="R2">
         <v>-121.3466079962483</v>
@@ -1240,16 +1240,16 @@
         <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>0.2400406981651698</v>
+        <v>0.2400406981651696</v>
       </c>
       <c r="P4">
-        <v>0.8960735770323205</v>
+        <v>0.8960735770323204</v>
       </c>
       <c r="Q4">
-        <v>5.766209886018101</v>
+        <v>5.766209886018099</v>
       </c>
       <c r="R4">
-        <v>-121.3466079469509</v>
+        <v>-121.346607946951</v>
       </c>
       <c r="S4">
         <v>173.4315681777209</v>
@@ -1296,16 +1296,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.020226441284735</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
         <v>0.2400406981658866</v>
       </c>
       <c r="P5">
-        <v>0.8960735770410369</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q5">
-        <v>5.766209886365067</v>
+        <v>5.766209886365068</v>
       </c>
       <c r="R5">
         <v>-121.3466079422891</v>
@@ -1358,13 +1358,13 @@
         <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>0.2400406981658867</v>
+        <v>0.2400406981658866</v>
       </c>
       <c r="P6">
-        <v>0.8960735770410367</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q6">
-        <v>5.766209886365059</v>
+        <v>5.766209886365068</v>
       </c>
       <c r="R6">
         <v>-121.3466079422891</v>
@@ -1453,19 +1453,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.734156921377197</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="D2">
-        <v>3.734156921377197</v>
+        <v>3.734156921377196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>237.1508154128772</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="G2">
-        <v>237.1508154128772</v>
+        <v>237.1508154128771</v>
       </c>
       <c r="H2">
         <v>1.324394477419386</v>
@@ -1474,13 +1474,13 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
@@ -1495,7 +1495,7 @@
         <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884997137</v>
+        <v>5.766209884997138</v>
       </c>
       <c r="R2">
         <v>-121.3466079962483</v>
@@ -1607,16 +1607,16 @@
         <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>0.2400406981651698</v>
+        <v>0.2400406981651696</v>
       </c>
       <c r="P4">
-        <v>0.8960735770323205</v>
+        <v>0.8960735770323204</v>
       </c>
       <c r="Q4">
-        <v>5.766209886018101</v>
+        <v>5.766209886018099</v>
       </c>
       <c r="R4">
-        <v>-121.3466079469509</v>
+        <v>-121.346607946951</v>
       </c>
       <c r="S4">
         <v>173.4315681777209</v>
@@ -1663,16 +1663,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.020226441284735</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
         <v>0.2400406981658866</v>
       </c>
       <c r="P5">
-        <v>0.8960735770410369</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q5">
-        <v>5.766209886365067</v>
+        <v>5.766209886365068</v>
       </c>
       <c r="R5">
         <v>-121.3466079422891</v>
@@ -1725,13 +1725,13 @@
         <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>0.2400406981658867</v>
+        <v>0.2400406981658866</v>
       </c>
       <c r="P6">
-        <v>0.8960735770410367</v>
+        <v>0.8960735770410365</v>
       </c>
       <c r="Q6">
-        <v>5.766209886365059</v>
+        <v>5.766209886365068</v>
       </c>
       <c r="R6">
         <v>-121.3466079422891</v>
@@ -1835,19 +1835,19 @@
         <v>230.9401157662428</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -1862,7 +1862,7 @@
         <v>0.8660254037849897</v>
       </c>
       <c r="Q2">
-        <v>1.720135230673776E-10</v>
+        <v>1.720167889283314E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -1912,22 +1912,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.8660254036789676</v>
+        <v>0.8660254036789677</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.8660254038905275</v>
+        <v>0.8660254038905277</v>
       </c>
       <c r="Q3">
-        <v>4.107325657298007E-10</v>
+        <v>4.107318871306543E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>179.9999999995807</v>
+        <v>179.9999999995806</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1971,22 +1971,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8660254036546304</v>
+        <v>0.8660254036546307</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.866025403914865</v>
+        <v>0.8660254039148652</v>
       </c>
       <c r="Q4">
-        <v>3.135437461079933E-09</v>
+        <v>3.135426825864409E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.999999996856</v>
+        <v>179.9999999968559</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8660254036465179</v>
+        <v>0.8660254036465181</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>0.8660254039229777</v>
       </c>
       <c r="Q5">
-        <v>4.043686462035157E-09</v>
+        <v>4.043658118464392E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2089,16 +2089,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8660254036465179</v>
+        <v>0.8660254036465181</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.8660254039229776</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q6">
-        <v>4.043673739804489E-09</v>
+        <v>4.043658118464392E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2202,19 +2202,19 @@
         <v>230.9401157662428</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -2229,7 +2229,7 @@
         <v>0.8660254037849897</v>
       </c>
       <c r="Q2">
-        <v>1.720135230673776E-10</v>
+        <v>1.720167889283314E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -2279,22 +2279,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.8660254036789676</v>
+        <v>0.8660254036789677</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.8660254038905275</v>
+        <v>0.8660254038905277</v>
       </c>
       <c r="Q3">
-        <v>4.107325657298007E-10</v>
+        <v>4.107318871306543E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>179.9999999995807</v>
+        <v>179.9999999995806</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2338,22 +2338,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8660254036546304</v>
+        <v>0.8660254036546307</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.866025403914865</v>
+        <v>0.8660254039148652</v>
       </c>
       <c r="Q4">
-        <v>3.135437461079933E-09</v>
+        <v>3.135426825864409E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.999999996856</v>
+        <v>179.9999999968559</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8660254036465179</v>
+        <v>0.8660254036465181</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -2406,7 +2406,7 @@
         <v>0.8660254039229777</v>
       </c>
       <c r="Q5">
-        <v>4.043686462035157E-09</v>
+        <v>4.043658118464392E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2456,16 +2456,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8660254036465179</v>
+        <v>0.8660254036465181</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.8660254039229776</v>
+        <v>0.8660254039229777</v>
       </c>
       <c r="Q6">
-        <v>4.043673739804489E-09</v>
+        <v>4.043658118464392E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2569,19 +2569,19 @@
         <v>194.0417843782413</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -2590,13 +2590,13 @@
         <v>0.9220324944339024</v>
       </c>
       <c r="O2">
-        <v>0.1964063473242863</v>
+        <v>0.1964063473242864</v>
       </c>
       <c r="P2">
         <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
-        <v>5.173976904115787</v>
+        <v>5.173976904115785</v>
       </c>
       <c r="R2">
         <v>-122.1449202961592</v>
@@ -2655,7 +2655,7 @@
         <v>0.8180121062689186</v>
       </c>
       <c r="Q3">
-        <v>5.173976904114591</v>
+        <v>5.173976904114592</v>
       </c>
       <c r="R3">
         <v>-122.1449202549969</v>
@@ -2705,16 +2705,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9220324943235482</v>
+        <v>0.9220324943235484</v>
       </c>
       <c r="O4">
-        <v>0.1964063472443389</v>
+        <v>0.196406347244339</v>
       </c>
       <c r="P4">
-        <v>0.8180121062966166</v>
+        <v>0.8180121062966169</v>
       </c>
       <c r="Q4">
-        <v>5.173976906219928</v>
+        <v>5.173976906219927</v>
       </c>
       <c r="R4">
         <v>-122.1449202329784</v>
@@ -2764,19 +2764,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9220324943163393</v>
+        <v>0.9220324943163395</v>
       </c>
       <c r="O5">
         <v>0.1964063472535607</v>
       </c>
       <c r="P5">
-        <v>0.8180121063058493</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q5">
-        <v>5.173976906921717</v>
+        <v>5.173976906921703</v>
       </c>
       <c r="R5">
-        <v>-122.1449202256389</v>
+        <v>-122.144920225639</v>
       </c>
       <c r="S5">
         <v>174.1659345837774</v>
@@ -2823,19 +2823,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9220324943163393</v>
+        <v>0.9220324943163395</v>
       </c>
       <c r="O6">
         <v>0.1964063472535607</v>
       </c>
       <c r="P6">
-        <v>0.8180121063058493</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q6">
-        <v>5.173976906921709</v>
+        <v>5.173976906921703</v>
       </c>
       <c r="R6">
-        <v>-122.1449202256389</v>
+        <v>-122.144920225639</v>
       </c>
       <c r="S6">
         <v>174.1659345837774</v>
@@ -2936,19 +2936,19 @@
         <v>194.0417843782413</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -2957,13 +2957,13 @@
         <v>0.9220324944339024</v>
       </c>
       <c r="O2">
-        <v>0.1964063473242863</v>
+        <v>0.1964063473242864</v>
       </c>
       <c r="P2">
         <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
-        <v>5.173976904115787</v>
+        <v>5.173976904115785</v>
       </c>
       <c r="R2">
         <v>-122.1449202961592</v>
@@ -3022,7 +3022,7 @@
         <v>0.8180121062689186</v>
       </c>
       <c r="Q3">
-        <v>5.173976904114591</v>
+        <v>5.173976904114592</v>
       </c>
       <c r="R3">
         <v>-122.1449202549969</v>
@@ -3072,16 +3072,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9220324943235482</v>
+        <v>0.9220324943235484</v>
       </c>
       <c r="O4">
-        <v>0.1964063472443389</v>
+        <v>0.196406347244339</v>
       </c>
       <c r="P4">
-        <v>0.8180121062966166</v>
+        <v>0.8180121062966169</v>
       </c>
       <c r="Q4">
-        <v>5.173976906219928</v>
+        <v>5.173976906219927</v>
       </c>
       <c r="R4">
         <v>-122.1449202329784</v>
@@ -3131,19 +3131,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9220324943163393</v>
+        <v>0.9220324943163395</v>
       </c>
       <c r="O5">
         <v>0.1964063472535607</v>
       </c>
       <c r="P5">
-        <v>0.8180121063058493</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q5">
-        <v>5.173976906921717</v>
+        <v>5.173976906921703</v>
       </c>
       <c r="R5">
-        <v>-122.1449202256389</v>
+        <v>-122.144920225639</v>
       </c>
       <c r="S5">
         <v>174.1659345837774</v>
@@ -3190,19 +3190,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9220324943163393</v>
+        <v>0.9220324943163395</v>
       </c>
       <c r="O6">
         <v>0.1964063472535607</v>
       </c>
       <c r="P6">
-        <v>0.8180121063058493</v>
+        <v>0.8180121063058495</v>
       </c>
       <c r="Q6">
-        <v>5.173976906921709</v>
+        <v>5.173976906921703</v>
       </c>
       <c r="R6">
-        <v>-122.1449202256389</v>
+        <v>-122.144920225639</v>
       </c>
       <c r="S6">
         <v>174.1659345837774</v>
@@ -3288,7 +3288,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5.248639108526413</v>
+        <v>5.248639108526411</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3297,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>333.3333522405614</v>
+        <v>333.3333522405613</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3312,13 +3312,13 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163437</v>
+        <v>1.324394473163436</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.32439447410434</v>
+        <v>1.324394474104339</v>
       </c>
       <c r="M2">
         <v>13.24394453563962</v>
@@ -3330,10 +3330,10 @@
         <v>1.100000023884843</v>
       </c>
       <c r="P2">
-        <v>0.6350853099409383</v>
+        <v>0.6350853099409386</v>
       </c>
       <c r="Q2">
-        <v>59.99999999685335</v>
+        <v>59.99999999685333</v>
       </c>
       <c r="R2">
         <v>-89.99999999999633</v>
@@ -3342,7 +3342,7 @@
         <v>119.9999999996536</v>
       </c>
       <c r="T2">
-        <v>5.248639108526412</v>
+        <v>5.24863910852641</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3386,19 +3386,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853099894115</v>
+        <v>0.6350853099894112</v>
       </c>
       <c r="O3">
         <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>0.6350853098300094</v>
+        <v>0.6350853098300102</v>
       </c>
       <c r="Q3">
-        <v>60.0000000023992</v>
+        <v>60.00000000239915</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999581</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S3">
         <v>120.0000000058974</v>
@@ -3448,19 +3448,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853100298055</v>
+        <v>0.6350853100298051</v>
       </c>
       <c r="O4">
         <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>0.6350853098168605</v>
+        <v>0.6350853098168617</v>
       </c>
       <c r="Q4">
-        <v>60.00000000166497</v>
+        <v>60.00000000166491</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S4">
         <v>120.0000000094205</v>
@@ -3510,19 +3510,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853100432701</v>
+        <v>0.6350853100432696</v>
       </c>
       <c r="O5">
         <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>0.6350853098124773</v>
+        <v>0.6350853098124788</v>
       </c>
       <c r="Q5">
-        <v>60.00000000142024</v>
+        <v>60.00000000142018</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S5">
         <v>120.0000000105949</v>
@@ -3572,22 +3572,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.63508531004327</v>
+        <v>0.6350853100432696</v>
       </c>
       <c r="O6">
         <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>0.6350853098124773</v>
+        <v>0.6350853098124788</v>
       </c>
       <c r="Q6">
-        <v>60.00000000142024</v>
+        <v>60.00000000142018</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S6">
-        <v>120.0000000105948</v>
+        <v>120.0000000105949</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -3673,7 +3673,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5.248639108526413</v>
+        <v>5.248639108526411</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>333.3333522405614</v>
+        <v>333.3333522405613</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3697,13 +3697,13 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163437</v>
+        <v>1.324394473163436</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.32439447410434</v>
+        <v>1.324394474104339</v>
       </c>
       <c r="M2">
         <v>13.24394453563962</v>
@@ -3715,10 +3715,10 @@
         <v>1.100000023884843</v>
       </c>
       <c r="P2">
-        <v>0.6350853099409383</v>
+        <v>0.6350853099409386</v>
       </c>
       <c r="Q2">
-        <v>59.99999999685335</v>
+        <v>59.99999999685333</v>
       </c>
       <c r="R2">
         <v>-89.99999999999633</v>
@@ -3727,7 +3727,7 @@
         <v>119.9999999996536</v>
       </c>
       <c r="T2">
-        <v>5.248639108526412</v>
+        <v>5.24863910852641</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3771,19 +3771,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853099894115</v>
+        <v>0.6350853099894112</v>
       </c>
       <c r="O3">
         <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>0.6350853098300094</v>
+        <v>0.6350853098300102</v>
       </c>
       <c r="Q3">
-        <v>60.0000000023992</v>
+        <v>60.00000000239915</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999581</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S3">
         <v>120.0000000058974</v>
@@ -3833,19 +3833,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853100298055</v>
+        <v>0.6350853100298051</v>
       </c>
       <c r="O4">
         <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>0.6350853098168605</v>
+        <v>0.6350853098168617</v>
       </c>
       <c r="Q4">
-        <v>60.00000000166497</v>
+        <v>60.00000000166491</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S4">
         <v>120.0000000094205</v>
@@ -3895,19 +3895,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853100432701</v>
+        <v>0.6350853100432696</v>
       </c>
       <c r="O5">
         <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>0.6350853098124773</v>
+        <v>0.6350853098124788</v>
       </c>
       <c r="Q5">
-        <v>60.00000000142024</v>
+        <v>60.00000000142018</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S5">
         <v>120.0000000105949</v>
@@ -3957,22 +3957,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.63508531004327</v>
+        <v>0.6350853100432696</v>
       </c>
       <c r="O6">
         <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>0.6350853098124773</v>
+        <v>0.6350853098124788</v>
       </c>
       <c r="Q6">
-        <v>60.00000000142024</v>
+        <v>60.00000000142018</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999582</v>
+        <v>-89.99999999999579</v>
       </c>
       <c r="S6">
-        <v>120.0000000105948</v>
+        <v>120.0000000105949</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -4082,13 +4082,13 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163437</v>
+        <v>1.324394473163436</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.32439447410434</v>
+        <v>1.324394474104339</v>
       </c>
       <c r="M2">
         <v>13.24394453563962</v>
@@ -4103,7 +4103,7 @@
         <v>0.8378427578966808</v>
       </c>
       <c r="Q2">
-        <v>40.40951795604944</v>
+        <v>40.40951795604943</v>
       </c>
       <c r="R2">
         <v>-89.99999999999652</v>
@@ -4156,19 +4156,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6918398877714428</v>
+        <v>0.6918398877714425</v>
       </c>
       <c r="O3">
         <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>0.8378427578167497</v>
+        <v>0.8378427578167503</v>
       </c>
       <c r="Q3">
-        <v>40.40951796258043</v>
+        <v>40.4095179625804</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
         <v>128.9574716984651</v>
@@ -4218,19 +4218,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6918398877978504</v>
+        <v>0.69183988779785</v>
       </c>
       <c r="O4">
         <v>1.100000023874165</v>
       </c>
       <c r="P4">
-        <v>0.8378427578056242</v>
+        <v>0.8378427578056251</v>
       </c>
       <c r="Q4">
-        <v>40.40951796344667</v>
+        <v>40.40951796344662</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
         <v>128.9574717002523</v>
@@ -4280,19 +4280,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6918398878066528</v>
+        <v>0.6918398878066526</v>
       </c>
       <c r="O5">
         <v>1.100000023874165</v>
       </c>
       <c r="P5">
-        <v>0.8378427578019155</v>
+        <v>0.8378427578019166</v>
       </c>
       <c r="Q5">
-        <v>40.40951796373541</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S5">
         <v>128.957471700848</v>
@@ -4342,19 +4342,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6918398878066528</v>
+        <v>0.6918398878066526</v>
       </c>
       <c r="O6">
         <v>1.100000023874165</v>
       </c>
       <c r="P6">
-        <v>0.8378427578019157</v>
+        <v>0.8378427578019166</v>
       </c>
       <c r="Q6">
-        <v>40.40951796373541</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S6">
         <v>128.957471700848</v>
@@ -4618,13 +4618,13 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163437</v>
+        <v>1.324394473163436</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
       </c>
       <c r="L2">
-        <v>1.32439447410434</v>
+        <v>1.324394474104339</v>
       </c>
       <c r="M2">
         <v>13.24394453563962</v>
@@ -4639,7 +4639,7 @@
         <v>0.8378427578966808</v>
       </c>
       <c r="Q2">
-        <v>40.40951795604944</v>
+        <v>40.40951795604943</v>
       </c>
       <c r="R2">
         <v>-89.99999999999652</v>
@@ -4692,19 +4692,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6918398877714428</v>
+        <v>0.6918398877714425</v>
       </c>
       <c r="O3">
         <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>0.8378427578167497</v>
+        <v>0.8378427578167503</v>
       </c>
       <c r="Q3">
-        <v>40.40951796258043</v>
+        <v>40.4095179625804</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
         <v>128.9574716984651</v>
@@ -4754,19 +4754,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6918398877978504</v>
+        <v>0.69183988779785</v>
       </c>
       <c r="O4">
         <v>1.100000023874165</v>
       </c>
       <c r="P4">
-        <v>0.8378427578056242</v>
+        <v>0.8378427578056251</v>
       </c>
       <c r="Q4">
-        <v>40.40951796344667</v>
+        <v>40.40951796344662</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
         <v>128.9574717002523</v>
@@ -4816,19 +4816,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6918398878066528</v>
+        <v>0.6918398878066526</v>
       </c>
       <c r="O5">
         <v>1.100000023874165</v>
       </c>
       <c r="P5">
-        <v>0.8378427578019155</v>
+        <v>0.8378427578019166</v>
       </c>
       <c r="Q5">
-        <v>40.40951796373541</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S5">
         <v>128.957471700848</v>
@@ -4878,19 +4878,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6918398878066528</v>
+        <v>0.6918398878066526</v>
       </c>
       <c r="O6">
         <v>1.100000023874165</v>
       </c>
       <c r="P6">
-        <v>0.8378427578019157</v>
+        <v>0.8378427578019166</v>
       </c>
       <c r="Q6">
-        <v>40.40951796373541</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999615</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S6">
         <v>128.957471700848</v>
@@ -4997,19 +4997,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976284</v>
+        <v>1.504993724976285</v>
       </c>
       <c r="I2">
-        <v>15.04993697142822</v>
+        <v>15.04993697142821</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648797</v>
       </c>
       <c r="K2">
         <v>15.04993697229388</v>
       </c>
       <c r="L2">
-        <v>1.50499372069543</v>
+        <v>1.504993720695428</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5077,19 +5077,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502692231758</v>
+        <v>0.5773502692231756</v>
       </c>
       <c r="O3">
-        <v>0.9999999999962955</v>
+        <v>0.9999999999962953</v>
       </c>
       <c r="P3">
-        <v>0.5773502691507324</v>
+        <v>0.5773502691507325</v>
       </c>
       <c r="Q3">
-        <v>60.00000000216501</v>
+        <v>60.000000002165</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S3">
         <v>120.0000000019794</v>
@@ -5139,19 +5139,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.5773502692712905</v>
+        <v>0.5773502692712903</v>
       </c>
       <c r="O4">
         <v>0.9999999999962953</v>
       </c>
       <c r="P4">
-        <v>0.5773502691501725</v>
+        <v>0.5773502691501728</v>
       </c>
       <c r="Q4">
         <v>59.99999999947237</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S4">
         <v>120.0000000074609</v>
@@ -5201,19 +5201,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.577350269287329</v>
+        <v>0.5773502692873287</v>
       </c>
       <c r="O5">
-        <v>0.9999999999962956</v>
+        <v>0.9999999999962953</v>
       </c>
       <c r="P5">
-        <v>0.5773502691499859</v>
+        <v>0.5773502691499862</v>
       </c>
       <c r="Q5">
-        <v>59.99999999857484</v>
+        <v>59.99999999857482</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999586</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S5">
         <v>120.000000009288</v>
@@ -5263,19 +5263,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502692873288</v>
+        <v>0.5773502692873287</v>
       </c>
       <c r="O6">
         <v>0.9999999999962953</v>
       </c>
       <c r="P6">
-        <v>0.5773502691499859</v>
+        <v>0.5773502691499862</v>
       </c>
       <c r="Q6">
-        <v>59.99999999857484</v>
+        <v>59.99999999857482</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S6">
         <v>120.000000009288</v>
@@ -5382,19 +5382,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976284</v>
+        <v>1.504993724976285</v>
       </c>
       <c r="I2">
-        <v>15.04993697142822</v>
+        <v>15.04993697142821</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648797</v>
       </c>
       <c r="K2">
         <v>15.04993697229388</v>
       </c>
       <c r="L2">
-        <v>1.50499372069543</v>
+        <v>1.504993720695428</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5462,19 +5462,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502692231758</v>
+        <v>0.5773502692231756</v>
       </c>
       <c r="O3">
-        <v>0.9999999999962955</v>
+        <v>0.9999999999962953</v>
       </c>
       <c r="P3">
-        <v>0.5773502691507324</v>
+        <v>0.5773502691507325</v>
       </c>
       <c r="Q3">
-        <v>60.00000000216501</v>
+        <v>60.000000002165</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S3">
         <v>120.0000000019794</v>
@@ -5524,19 +5524,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.5773502692712905</v>
+        <v>0.5773502692712903</v>
       </c>
       <c r="O4">
         <v>0.9999999999962953</v>
       </c>
       <c r="P4">
-        <v>0.5773502691501725</v>
+        <v>0.5773502691501728</v>
       </c>
       <c r="Q4">
         <v>59.99999999947237</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S4">
         <v>120.0000000074609</v>
@@ -5586,19 +5586,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.577350269287329</v>
+        <v>0.5773502692873287</v>
       </c>
       <c r="O5">
-        <v>0.9999999999962956</v>
+        <v>0.9999999999962953</v>
       </c>
       <c r="P5">
-        <v>0.5773502691499859</v>
+        <v>0.5773502691499862</v>
       </c>
       <c r="Q5">
-        <v>59.99999999857484</v>
+        <v>59.99999999857482</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999586</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S5">
         <v>120.000000009288</v>
@@ -5648,19 +5648,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502692873288</v>
+        <v>0.5773502692873287</v>
       </c>
       <c r="O6">
         <v>0.9999999999962953</v>
       </c>
       <c r="P6">
-        <v>0.5773502691499859</v>
+        <v>0.5773502691499862</v>
       </c>
       <c r="Q6">
-        <v>59.99999999857484</v>
+        <v>59.99999999857482</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999585</v>
+        <v>-89.99999999999584</v>
       </c>
       <c r="S6">
         <v>120.000000009288</v>
@@ -5767,19 +5767,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976284</v>
+        <v>1.504993724976285</v>
       </c>
       <c r="I2">
-        <v>15.04993697142822</v>
+        <v>15.04993697142821</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648797</v>
       </c>
       <c r="K2">
         <v>15.04993697229388</v>
       </c>
       <c r="L2">
-        <v>1.50499372069543</v>
+        <v>1.504993720695428</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5791,7 +5791,7 @@
         <v>0.9999999999908641</v>
       </c>
       <c r="P2">
-        <v>0.7472997527351807</v>
+        <v>0.7472997527351806</v>
       </c>
       <c r="Q2">
         <v>41.77463363119256</v>
@@ -5847,22 +5847,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6184267550404211</v>
+        <v>0.6184267550404209</v>
       </c>
       <c r="O3">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P3">
-        <v>0.747299752657798</v>
+        <v>0.7472997526577979</v>
       </c>
       <c r="Q3">
-        <v>41.77463363810636</v>
+        <v>41.77463363810635</v>
       </c>
       <c r="R3">
         <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>128.1091583228107</v>
+        <v>128.1091583228108</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -5909,16 +5909,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6184267550800499</v>
+        <v>0.6184267550800497</v>
       </c>
       <c r="O4">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P4">
         <v>0.7472997526545254</v>
       </c>
       <c r="Q4">
-        <v>41.77463363817496</v>
+        <v>41.77463363817495</v>
       </c>
       <c r="R4">
         <v>-89.99999999999615</v>
@@ -5971,19 +5971,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O5">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P5">
-        <v>0.7472997526534344</v>
+        <v>0.7472997526534345</v>
       </c>
       <c r="Q5">
-        <v>41.77463363819785</v>
+        <v>41.77463363819783</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999616</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S5">
         <v>128.1091583268488</v>
@@ -6033,19 +6033,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O6">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P6">
-        <v>0.7472997526534344</v>
+        <v>0.7472997526534345</v>
       </c>
       <c r="Q6">
-        <v>41.77463363819784</v>
+        <v>41.77463363819783</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999616</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S6">
         <v>128.1091583268488</v>
@@ -6152,19 +6152,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976284</v>
+        <v>1.504993724976285</v>
       </c>
       <c r="I2">
-        <v>15.04993697142822</v>
+        <v>15.04993697142821</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648797</v>
       </c>
       <c r="K2">
         <v>15.04993697229388</v>
       </c>
       <c r="L2">
-        <v>1.50499372069543</v>
+        <v>1.504993720695428</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -6176,7 +6176,7 @@
         <v>0.9999999999908641</v>
       </c>
       <c r="P2">
-        <v>0.7472997527351807</v>
+        <v>0.7472997527351806</v>
       </c>
       <c r="Q2">
         <v>41.77463363119256</v>
@@ -6232,22 +6232,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6184267550404211</v>
+        <v>0.6184267550404209</v>
       </c>
       <c r="O3">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P3">
-        <v>0.747299752657798</v>
+        <v>0.7472997526577979</v>
       </c>
       <c r="Q3">
-        <v>41.77463363810636</v>
+        <v>41.77463363810635</v>
       </c>
       <c r="R3">
         <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>128.1091583228107</v>
+        <v>128.1091583228108</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -6294,16 +6294,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6184267550800499</v>
+        <v>0.6184267550800497</v>
       </c>
       <c r="O4">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P4">
         <v>0.7472997526545254</v>
       </c>
       <c r="Q4">
-        <v>41.77463363817496</v>
+        <v>41.77463363817495</v>
       </c>
       <c r="R4">
         <v>-89.99999999999615</v>
@@ -6356,19 +6356,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O5">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P5">
-        <v>0.7472997526534344</v>
+        <v>0.7472997526534345</v>
       </c>
       <c r="Q5">
-        <v>41.77463363819785</v>
+        <v>41.77463363819783</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999616</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S5">
         <v>128.1091583268488</v>
@@ -6418,19 +6418,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O6">
-        <v>0.9999999999908707</v>
+        <v>0.9999999999908705</v>
       </c>
       <c r="P6">
-        <v>0.7472997526534344</v>
+        <v>0.7472997526534345</v>
       </c>
       <c r="Q6">
-        <v>41.77463363819784</v>
+        <v>41.77463363819783</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999616</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S6">
         <v>128.1091583268488</v>
@@ -6525,7 +6525,7 @@
         <v>5.248639108736852</v>
       </c>
       <c r="D2">
-        <v>5.248639107970818</v>
+        <v>5.248639107970816</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -6534,7 +6534,7 @@
         <v>333.3333522539261</v>
       </c>
       <c r="G2">
-        <v>333.3333522052764</v>
+        <v>333.3333522052763</v>
       </c>
       <c r="H2">
         <v>1.324394477419386</v>
@@ -6543,28 +6543,28 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.6350853098347081</v>
+        <v>0.6350853098347083</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098507079</v>
+        <v>0.635085309850708</v>
       </c>
       <c r="Q2">
-        <v>-4.877412548010482E-09</v>
+        <v>-4.877415051309047E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6573,7 +6573,7 @@
         <v>179.999999996043</v>
       </c>
       <c r="T2">
-        <v>5.24863910842028</v>
+        <v>5.248639108420279</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6617,16 +6617,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853097237735</v>
+        <v>0.6350853097237741</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.6350853099661087</v>
+        <v>0.6350853099661088</v>
       </c>
       <c r="Q3">
-        <v>1.367294711046319E-09</v>
+        <v>1.367259943169384E-09</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -6679,16 +6679,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853097106247</v>
+        <v>0.6350853097106254</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6350853100065024</v>
+        <v>0.6350853100065026</v>
       </c>
       <c r="Q4">
-        <v>4.890429623046234E-09</v>
+        <v>4.890383728000621E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -6741,16 +6741,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853097062418</v>
+        <v>0.6350853097062424</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.635085310019967</v>
+        <v>0.6350853100199672</v>
       </c>
       <c r="Q5">
-        <v>6.064796072658097E-09</v>
+        <v>6.064748332970874E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -6803,16 +6803,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853097062419</v>
+        <v>0.6350853097062424</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.6350853100199668</v>
+        <v>0.6350853100199672</v>
       </c>
       <c r="Q6">
-        <v>6.064794416666137E-09</v>
+        <v>6.064748332970874E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -6910,7 +6910,7 @@
         <v>5.248639108736852</v>
       </c>
       <c r="D2">
-        <v>5.248639107970818</v>
+        <v>5.248639107970816</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -6919,7 +6919,7 @@
         <v>333.3333522539261</v>
       </c>
       <c r="G2">
-        <v>333.3333522052764</v>
+        <v>333.3333522052763</v>
       </c>
       <c r="H2">
         <v>1.324394477419386</v>
@@ -6928,28 +6928,28 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.6350853098347081</v>
+        <v>0.6350853098347083</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098507079</v>
+        <v>0.635085309850708</v>
       </c>
       <c r="Q2">
-        <v>-4.877412548010482E-09</v>
+        <v>-4.877415051309047E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6958,7 +6958,7 @@
         <v>179.999999996043</v>
       </c>
       <c r="T2">
-        <v>5.24863910842028</v>
+        <v>5.248639108420279</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -7002,16 +7002,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853097237735</v>
+        <v>0.6350853097237741</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.6350853099661087</v>
+        <v>0.6350853099661088</v>
       </c>
       <c r="Q3">
-        <v>1.367294711046319E-09</v>
+        <v>1.367259943169384E-09</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -7064,16 +7064,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853097106247</v>
+        <v>0.6350853097106254</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6350853100065024</v>
+        <v>0.6350853100065026</v>
       </c>
       <c r="Q4">
-        <v>4.890429623046234E-09</v>
+        <v>4.890383728000621E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -7126,16 +7126,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853097062418</v>
+        <v>0.6350853097062424</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.635085310019967</v>
+        <v>0.6350853100199672</v>
       </c>
       <c r="Q5">
-        <v>6.064796072658097E-09</v>
+        <v>6.064748332970874E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -7188,16 +7188,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853097062419</v>
+        <v>0.6350853097062424</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.6350853100199668</v>
+        <v>0.6350853100199672</v>
       </c>
       <c r="Q6">
-        <v>6.064794416666137E-09</v>
+        <v>6.064748332970874E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -7295,13 +7295,13 @@
         <v>3.617960382593723</v>
       </c>
       <c r="D2">
-        <v>3.617960382231208</v>
+        <v>3.617960382231207</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>229.7713440888677</v>
+        <v>229.7713440888676</v>
       </c>
       <c r="G2">
         <v>229.7713440658448</v>
@@ -7313,25 +7313,25 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.8378427578256962</v>
+        <v>0.8378427578256959</v>
       </c>
       <c r="O2">
-        <v>0.4028253111898907</v>
+        <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398877011792</v>
+        <v>0.6918398877011793</v>
       </c>
       <c r="Q2">
         <v>8.9574716935048</v>
@@ -7390,16 +7390,16 @@
         <v>0.8378427577457513</v>
       </c>
       <c r="O3">
-        <v>0.4028253110952159</v>
+        <v>0.4028253110952157</v>
       </c>
       <c r="P3">
-        <v>0.6918398877448082</v>
+        <v>0.6918398877448086</v>
       </c>
       <c r="Q3">
-        <v>8.957471696351691</v>
+        <v>8.957471696351671</v>
       </c>
       <c r="R3">
-        <v>-115.8807585788046</v>
+        <v>-115.8807585788045</v>
       </c>
       <c r="S3">
         <v>160.4095179634873</v>
@@ -7449,22 +7449,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.837842757734626</v>
+        <v>0.8378427577346259</v>
       </c>
       <c r="O4">
         <v>0.4028253110970204</v>
       </c>
       <c r="P4">
-        <v>0.6918398877712157</v>
+        <v>0.691839887771216</v>
       </c>
       <c r="Q4">
-        <v>8.957471698138875</v>
+        <v>8.95747169813885</v>
       </c>
       <c r="R4">
-        <v>-115.8807585718119</v>
+        <v>-115.8807585718118</v>
       </c>
       <c r="S4">
-        <v>160.4095179643536</v>
+        <v>160.4095179643535</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -7511,16 +7511,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8378427577309173</v>
+        <v>0.8378427577309175</v>
       </c>
       <c r="O5">
-        <v>0.4028253110976217</v>
+        <v>0.4028253110976218</v>
       </c>
       <c r="P5">
-        <v>0.6918398877800181</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q5">
-        <v>8.957471698734594</v>
+        <v>8.957471698734574</v>
       </c>
       <c r="R5">
         <v>-115.8807585694809</v>
@@ -7573,16 +7573,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8378427577309173</v>
+        <v>0.8378427577309175</v>
       </c>
       <c r="O6">
-        <v>0.4028253110976219</v>
+        <v>0.4028253110976218</v>
       </c>
       <c r="P6">
-        <v>0.691839887780018</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q6">
-        <v>8.957471698734588</v>
+        <v>8.957471698734574</v>
       </c>
       <c r="R6">
         <v>-115.8807585694809</v>
@@ -7680,13 +7680,13 @@
         <v>3.617960382593723</v>
       </c>
       <c r="D2">
-        <v>3.617960382231208</v>
+        <v>3.617960382231207</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>229.7713440888677</v>
+        <v>229.7713440888676</v>
       </c>
       <c r="G2">
         <v>229.7713440658448</v>
@@ -7698,25 +7698,25 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
       </c>
       <c r="N2">
-        <v>0.8378427578256962</v>
+        <v>0.8378427578256959</v>
       </c>
       <c r="O2">
-        <v>0.4028253111898907</v>
+        <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398877011792</v>
+        <v>0.6918398877011793</v>
       </c>
       <c r="Q2">
         <v>8.9574716935048</v>
@@ -7775,16 +7775,16 @@
         <v>0.8378427577457513</v>
       </c>
       <c r="O3">
-        <v>0.4028253110952159</v>
+        <v>0.4028253110952157</v>
       </c>
       <c r="P3">
-        <v>0.6918398877448082</v>
+        <v>0.6918398877448086</v>
       </c>
       <c r="Q3">
-        <v>8.957471696351691</v>
+        <v>8.957471696351671</v>
       </c>
       <c r="R3">
-        <v>-115.8807585788046</v>
+        <v>-115.8807585788045</v>
       </c>
       <c r="S3">
         <v>160.4095179634873</v>
@@ -7834,22 +7834,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.837842757734626</v>
+        <v>0.8378427577346259</v>
       </c>
       <c r="O4">
         <v>0.4028253110970204</v>
       </c>
       <c r="P4">
-        <v>0.6918398877712157</v>
+        <v>0.691839887771216</v>
       </c>
       <c r="Q4">
-        <v>8.957471698138875</v>
+        <v>8.95747169813885</v>
       </c>
       <c r="R4">
-        <v>-115.8807585718119</v>
+        <v>-115.8807585718118</v>
       </c>
       <c r="S4">
-        <v>160.4095179643536</v>
+        <v>160.4095179643535</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -7896,16 +7896,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8378427577309173</v>
+        <v>0.8378427577309175</v>
       </c>
       <c r="O5">
-        <v>0.4028253110976217</v>
+        <v>0.4028253110976218</v>
       </c>
       <c r="P5">
-        <v>0.6918398877800181</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q5">
-        <v>8.957471698734594</v>
+        <v>8.957471698734574</v>
       </c>
       <c r="R5">
         <v>-115.8807585694809</v>
@@ -7958,16 +7958,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8378427577309173</v>
+        <v>0.8378427577309175</v>
       </c>
       <c r="O6">
-        <v>0.4028253110976219</v>
+        <v>0.4028253110976218</v>
       </c>
       <c r="P6">
-        <v>0.691839887780018</v>
+        <v>0.6918398877800185</v>
       </c>
       <c r="Q6">
-        <v>8.957471698734588</v>
+        <v>8.957471698734574</v>
       </c>
       <c r="R6">
         <v>-115.8807585694809</v>
@@ -8062,7 +8062,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.198911196109218</v>
+        <v>4.198911196109217</v>
       </c>
       <c r="D2">
         <v>4.198911195412805</v>
@@ -8071,25 +8071,25 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>266.666676031469</v>
+        <v>266.6666760314689</v>
       </c>
       <c r="G2">
         <v>266.6666759872408</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -8101,10 +8101,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691743764</v>
+        <v>0.5773502691743765</v>
       </c>
       <c r="Q2">
-        <v>-5.812880099584224E-09</v>
+        <v>-5.812875646951555E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -8157,16 +8157,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502690917838</v>
+        <v>0.577350269091784</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.5773502692819927</v>
+        <v>0.577350269281993</v>
       </c>
       <c r="Q3">
-        <v>5.928701121525565E-10</v>
+        <v>5.928687968146642E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8219,16 +8219,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.577350269091224</v>
+        <v>0.5773502690912243</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.5773502693301076</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>6.074349654285723E-09</v>
+        <v>6.07433511756549E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -8281,22 +8281,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.5773502690910374</v>
+        <v>0.5773502690910377</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.577350269346146</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q5">
-        <v>7.90155864512457E-09</v>
+        <v>7.901497720967717E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -8343,22 +8343,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502690910373</v>
+        <v>0.5773502690910377</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.5773502693461458</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>7.901535153381744E-09</v>
+        <v>7.901497720967717E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -8598,7 +8598,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.198911196109218</v>
+        <v>4.198911196109217</v>
       </c>
       <c r="D2">
         <v>4.198911195412805</v>
@@ -8607,25 +8607,25 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>266.666676031469</v>
+        <v>266.6666760314689</v>
       </c>
       <c r="G2">
         <v>266.6666759872408</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -8637,10 +8637,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691743764</v>
+        <v>0.5773502691743765</v>
       </c>
       <c r="Q2">
-        <v>-5.812880099584224E-09</v>
+        <v>-5.812875646951555E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -8693,16 +8693,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502690917838</v>
+        <v>0.577350269091784</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.5773502692819927</v>
+        <v>0.577350269281993</v>
       </c>
       <c r="Q3">
-        <v>5.928701121525565E-10</v>
+        <v>5.928687968146642E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8755,16 +8755,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.577350269091224</v>
+        <v>0.5773502690912243</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.5773502693301076</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>6.074349654285723E-09</v>
+        <v>6.07433511756549E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -8817,22 +8817,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.5773502690910374</v>
+        <v>0.5773502690910377</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.577350269346146</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q5">
-        <v>7.90155864512457E-09</v>
+        <v>7.901497720967717E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -8879,22 +8879,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502690910373</v>
+        <v>0.5773502690910377</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.5773502693461458</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>7.901535153381744E-09</v>
+        <v>7.901497720967717E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -8983,7 +8983,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138951925</v>
+        <v>3.012913138951924</v>
       </c>
       <c r="D2">
         <v>3.012913138593917</v>
@@ -8992,43 +8992,43 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.345683300074</v>
+        <v>191.3456833000739</v>
       </c>
       <c r="G2">
-        <v>191.3456832773375</v>
+        <v>191.3456832773374</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.7472997527192562</v>
+        <v>0.7472997527192564</v>
       </c>
       <c r="O2">
         <v>0.3354590831689601</v>
       </c>
       <c r="P2">
-        <v>0.6184267550384411</v>
+        <v>0.6184267550384416</v>
       </c>
       <c r="Q2">
-        <v>8.109158318802287</v>
+        <v>8.109158318802297</v>
       </c>
       <c r="R2">
-        <v>-117.0248837767962</v>
+        <v>-117.0248837767961</v>
       </c>
       <c r="S2">
         <v>161.7746336318227</v>
@@ -9078,22 +9078,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.7472997526418613</v>
+        <v>0.7472997526418617</v>
       </c>
       <c r="O3">
         <v>0.3354590830770569</v>
       </c>
       <c r="P3">
-        <v>0.6184267550841054</v>
+        <v>0.6184267550841057</v>
       </c>
       <c r="Q3">
-        <v>8.109158321931387</v>
+        <v>8.109158321931394</v>
       </c>
       <c r="R3">
-        <v>-117.0248837562166</v>
+        <v>-117.0248837562165</v>
       </c>
       <c r="S3">
-        <v>161.7746336387372</v>
+        <v>161.7746336387373</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -9143,13 +9143,13 @@
         <v>0.7472997526385891</v>
       </c>
       <c r="O4">
-        <v>0.3354590831006831</v>
+        <v>0.335459083100683</v>
       </c>
       <c r="P4">
-        <v>0.6184267551237344</v>
+        <v>0.6184267551237347</v>
       </c>
       <c r="Q4">
-        <v>8.109158324959907</v>
+        <v>8.109158324959902</v>
       </c>
       <c r="R4">
         <v>-117.0248837452073</v>
@@ -9202,22 +9202,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.7472997526374979</v>
+        <v>0.747299752637498</v>
       </c>
       <c r="O5">
-        <v>0.3354590831085587</v>
+        <v>0.3354590831085583</v>
       </c>
       <c r="P5">
-        <v>0.618426755136944</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>8.10915832596941</v>
+        <v>8.109158325969403</v>
       </c>
       <c r="R5">
         <v>-117.0248837415376</v>
       </c>
       <c r="S5">
-        <v>161.7746336388287</v>
+        <v>161.7746336388288</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -9264,16 +9264,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.7472997526374978</v>
+        <v>0.747299752637498</v>
       </c>
       <c r="O6">
-        <v>0.3354590831085584</v>
+        <v>0.3354590831085583</v>
       </c>
       <c r="P6">
-        <v>0.6184267551369439</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q6">
-        <v>8.10915832596941</v>
+        <v>8.109158325969403</v>
       </c>
       <c r="R6">
         <v>-117.0248837415376</v>
@@ -9368,7 +9368,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138951925</v>
+        <v>3.012913138951924</v>
       </c>
       <c r="D2">
         <v>3.012913138593917</v>
@@ -9377,43 +9377,43 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.345683300074</v>
+        <v>191.3456833000739</v>
       </c>
       <c r="G2">
-        <v>191.3456832773375</v>
+        <v>191.3456832773374</v>
       </c>
       <c r="H2">
-        <v>1.504993724976225</v>
+        <v>1.504993724976226</v>
       </c>
       <c r="I2">
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246245</v>
+        <v>1.504993721246246</v>
       </c>
       <c r="K2">
-        <v>15.04993697324838</v>
+        <v>15.04993697324839</v>
       </c>
       <c r="L2">
-        <v>1.5049937206953</v>
+        <v>1.504993720695297</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.7472997527192562</v>
+        <v>0.7472997527192564</v>
       </c>
       <c r="O2">
         <v>0.3354590831689601</v>
       </c>
       <c r="P2">
-        <v>0.6184267550384411</v>
+        <v>0.6184267550384416</v>
       </c>
       <c r="Q2">
-        <v>8.109158318802287</v>
+        <v>8.109158318802297</v>
       </c>
       <c r="R2">
-        <v>-117.0248837767962</v>
+        <v>-117.0248837767961</v>
       </c>
       <c r="S2">
         <v>161.7746336318227</v>
@@ -9463,22 +9463,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.7472997526418613</v>
+        <v>0.7472997526418617</v>
       </c>
       <c r="O3">
         <v>0.3354590830770569</v>
       </c>
       <c r="P3">
-        <v>0.6184267550841054</v>
+        <v>0.6184267550841057</v>
       </c>
       <c r="Q3">
-        <v>8.109158321931387</v>
+        <v>8.109158321931394</v>
       </c>
       <c r="R3">
-        <v>-117.0248837562166</v>
+        <v>-117.0248837562165</v>
       </c>
       <c r="S3">
-        <v>161.7746336387372</v>
+        <v>161.7746336387373</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -9528,13 +9528,13 @@
         <v>0.7472997526385891</v>
       </c>
       <c r="O4">
-        <v>0.3354590831006831</v>
+        <v>0.335459083100683</v>
       </c>
       <c r="P4">
-        <v>0.6184267551237344</v>
+        <v>0.6184267551237347</v>
       </c>
       <c r="Q4">
-        <v>8.109158324959907</v>
+        <v>8.109158324959902</v>
       </c>
       <c r="R4">
         <v>-117.0248837452073</v>
@@ -9587,22 +9587,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.7472997526374979</v>
+        <v>0.747299752637498</v>
       </c>
       <c r="O5">
-        <v>0.3354590831085587</v>
+        <v>0.3354590831085583</v>
       </c>
       <c r="P5">
-        <v>0.618426755136944</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>8.10915832596941</v>
+        <v>8.109158325969403</v>
       </c>
       <c r="R5">
         <v>-117.0248837415376</v>
       </c>
       <c r="S5">
-        <v>161.7746336388287</v>
+        <v>161.7746336388288</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -9649,16 +9649,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.7472997526374978</v>
+        <v>0.747299752637498</v>
       </c>
       <c r="O6">
-        <v>0.3354590831085584</v>
+        <v>0.3354590831085583</v>
       </c>
       <c r="P6">
-        <v>0.6184267551369439</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q6">
-        <v>8.10915832596941</v>
+        <v>8.109158325969403</v>
       </c>
       <c r="R6">
         <v>-117.0248837415376</v>
@@ -10526,13 +10526,13 @@
         <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186056</v>
+        <v>1.324394474186054</v>
       </c>
       <c r="K2">
-        <v>13.24394453578228</v>
+        <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104236</v>
+        <v>1.324394474104235</v>
       </c>
       <c r="M2">
         <v>13.24394453563988</v>
@@ -10547,7 +10547,7 @@
         <v>0.9526279647833882</v>
       </c>
       <c r="Q2">
-        <v>-8.692030605078384E-11</v>
+        <v>-8.69272151632366E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -10597,16 +10597,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9526279646671955</v>
+        <v>0.9526279646671957</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.9526279648965608</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>1.457878492964093E-10</v>
+        <v>1.457724166160542E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -10656,16 +10656,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279646404242</v>
+        <v>0.9526279646404244</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279649233321</v>
+        <v>0.9526279649233318</v>
       </c>
       <c r="Q4">
-        <v>1.564915676528601E-09</v>
+        <v>1.564897976846374E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -10715,22 +10715,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9526279646315002</v>
+        <v>0.9526279646315007</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279649322559</v>
+        <v>0.9526279649322554</v>
       </c>
       <c r="Q5">
-        <v>2.037958276970909E-09</v>
+        <v>2.037934891115733E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999979535</v>
+        <v>179.9999999979534</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -10774,16 +10774,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9526279646315001</v>
+        <v>0.9526279646315007</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.9526279649322557</v>
+        <v>0.9526279649322554</v>
       </c>
       <c r="Q6">
-        <v>2.03795072457894E-09</v>
+        <v>2.037934891115733E-09</v>
       </c>
       <c r="R6">
         <v>0</v>

</xml_diff>